<commit_message>
add integration test cases
</commit_message>
<xml_diff>
--- a/Documents/2_BugReports/BugReports.xlsx
+++ b/Documents/2_BugReports/BugReports.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Automation\OrangeHRM---Automation-Java-Playwright-JUnit-\Documents\2_BugReports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B4DC00-42F0-4B96-B5FD-D9336B1586A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC16C94-31EE-4C20-8530-3A7E1B37AE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>Actual Result</t>
   </si>
   <si>
-    <t>Severity / Priority</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>Register_TC05</t>
+  </si>
+  <si>
+    <t>Severity</t>
   </si>
 </sst>
 </file>
@@ -241,7 +241,7 @@
     <tableColumn id="4" xr3:uid="{F99FE8E2-6D41-4518-BB68-A517A8B0605C}" name="Steps to Reproduce" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{470E75A5-1985-443E-BE34-54601ACB1601}" name="Expected Result" dataDxfId="6"/>
     <tableColumn id="6" xr3:uid="{DFF12385-8E17-4397-9392-2870CD680315}" name="Actual Result" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{54A479A2-F772-4A38-8F43-4AD63EE4EA5E}" name="Severity / Priority" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{54A479A2-F772-4A38-8F43-4AD63EE4EA5E}" name="Severity" dataDxfId="4"/>
     <tableColumn id="8" xr3:uid="{2BC9C6C1-B182-4FA5-BD30-741CE50EA1F3}" name="Status" dataDxfId="3"/>
     <tableColumn id="9" xr3:uid="{157EB1E8-9A4B-4561-8380-ACEC7D389FEF}" name="Environment" dataDxfId="2"/>
     <tableColumn id="10" xr3:uid="{E905AE30-6B62-4BFA-89CF-16AD40270BAD}" name="Fixed In Version" dataDxfId="1"/>
@@ -539,7 +539,7 @@
   <dimension ref="B2:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +559,7 @@
     <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,106 +579,106 @@
         <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="120" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="75" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="120" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="I5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>